<commit_message>
Updated metadata extract document
</commit_message>
<xml_diff>
--- a/Files/DataPass/Metadata.xlsx
+++ b/Files/DataPass/Metadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -102,6 +102,33 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Customer City</t>
+  </si>
+  <si>
+    <t>Customer State</t>
+  </si>
+  <si>
+    <t>Color_1</t>
+  </si>
+  <si>
+    <t>Color_2</t>
+  </si>
+  <si>
+    <t>Color_3</t>
+  </si>
+  <si>
+    <t>School_Mascot</t>
   </si>
 </sst>
 </file>
@@ -468,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C24"/>
+  <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,9 +506,11 @@
     <col min="1" max="1" width="45.109375" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -491,8 +520,11 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -500,7 +532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -511,7 +543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -522,7 +554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -530,7 +562,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -538,7 +570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -546,7 +578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -554,7 +586,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -562,7 +594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -570,7 +602,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -578,7 +610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -586,7 +618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -594,7 +626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -602,7 +634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -610,7 +642,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -618,7 +650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -626,7 +658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -634,7 +666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -642,7 +674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,8 +684,11 @@
       <c r="C21" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -661,7 +696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -669,11 +704,75 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial package data and updates to metadata spreadsheet
</commit_message>
<xml_diff>
--- a/Files/DataPass/Metadata.xlsx
+++ b/Files/DataPass/Metadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +129,93 @@
   </si>
   <si>
     <t>School_Mascot</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>AffiLIATION_BY_USE</t>
+  </si>
+  <si>
+    <t>Base_Color</t>
+  </si>
+  <si>
+    <t>color1</t>
+  </si>
+  <si>
+    <t>color2</t>
+  </si>
+  <si>
+    <t>color3</t>
+  </si>
+  <si>
+    <t>color4</t>
+  </si>
+  <si>
+    <t>color5</t>
+  </si>
+  <si>
+    <t>color6</t>
+  </si>
+  <si>
+    <t>color7</t>
+  </si>
+  <si>
+    <t>color8</t>
+  </si>
+  <si>
+    <t>color9</t>
+  </si>
+  <si>
+    <t>color10</t>
+  </si>
+  <si>
+    <t>color_scheme</t>
+  </si>
+  <si>
+    <t>customer_historic_use_color</t>
+  </si>
+  <si>
+    <t>customer_historic_use_design</t>
+  </si>
+  <si>
+    <t>status_life_cycle</t>
+  </si>
+  <si>
+    <t>status_cataloging</t>
+  </si>
+  <si>
+    <t>status_availability</t>
+  </si>
+  <si>
+    <t>Set to Quarantineed</t>
+  </si>
+  <si>
+    <t>Base_Color_Tones</t>
+  </si>
+  <si>
+    <t>Enhancement_color</t>
+  </si>
+  <si>
+    <t>business_default_use</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1g</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>Customer Default - Use this image when displaying customers - Look for crest, logo, mascot in that order</t>
+  </si>
+  <si>
+    <t>status_automation</t>
   </si>
 </sst>
 </file>
@@ -172,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -180,6 +267,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F32"/>
+  <dimension ref="A2:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,10 +600,11 @@
     <col min="2" max="2" width="12.77734375" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="18.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="37.44140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -523,8 +617,12 @@
       <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -532,7 +630,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -543,7 +641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -554,15 +652,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -570,7 +671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -578,7 +679,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -586,7 +687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -594,7 +695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -602,7 +703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -610,7 +711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -618,7 +719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -626,7 +727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -634,7 +735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -642,7 +743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -650,7 +751,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -658,7 +759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -666,7 +767,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -674,7 +775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,16 +788,22 @@
       <c r="D21" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -704,7 +811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -712,15 +819,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -728,7 +838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -736,7 +846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -744,7 +854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -752,7 +862,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -760,7 +870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -768,11 +878,225 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>